<commit_message>
<MS 2/10> Approved (working version of Reports amend)
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -15,17 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="25">
-  <si>
-    <t>Andrew Limited</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>test.test@test.com</t>
   </si>
   <si>
-    <t>07111111111</t>
-  </si>
-  <si>
     <t>Neilarmstrong Street</t>
   </si>
   <si>
@@ -41,9 +35,6 @@
     <t>Andrews</t>
   </si>
   <si>
-    <t>11111111111</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -83,13 +74,16 @@
     <t>Once we receive your signed application, assuming all is ok, we will open the account and advise you of your account number.</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Header</t>
+  </si>
+  <si>
+    <t>St Andrew Limited</t>
+  </si>
+  <si>
+    <t>07111234111</t>
+  </si>
+  <si>
+    <t>123456789</t>
   </si>
 </sst>
 </file>
@@ -444,80 +438,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="K2" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -527,11 +521,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -540,83 +532,76 @@
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<MS 2/10> Approved. Customised Timestamp code
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Intro_0" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -27,9 +27,6 @@
   </si>
   <si>
     <t>Montebello</t>
-  </si>
-  <si>
-    <t>E13 6SE</t>
   </si>
   <si>
     <t>Andrews</t>
@@ -438,80 +435,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -523,7 +520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -536,54 +535,54 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
@@ -594,14 +593,12 @@
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<MS 2/11> Approved (Header Images in Xpath)
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805"/>
   </bookViews>
   <sheets>
     <sheet name="Intro_0" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>123456789</t>
+  </si>
+  <si>
+    <t>E126SE</t>
   </si>
 </sst>
 </file>
@@ -435,8 +438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -520,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -593,7 +596,9 @@
       <c r="H2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
<MS 2/14> Approved (Excel Iteration Sample)
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Intro_0" sheetId="4" r:id="rId1"/>
     <sheet name="BD_1" sheetId="1" r:id="rId2"/>
+    <sheet name="sample" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -84,6 +85,42 @@
   </si>
   <si>
     <t>E126SE</t>
+  </si>
+  <si>
+    <t>TC001</t>
+  </si>
+  <si>
+    <t>TC002</t>
+  </si>
+  <si>
+    <t>987654321</t>
+  </si>
+  <si>
+    <t>merlin.samuel@gmail.com</t>
+  </si>
+  <si>
+    <t>06245678756</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Austin Woods</t>
+  </si>
+  <si>
+    <t>Charlotte</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>90640</t>
+  </si>
+  <si>
+    <t>Merlin</t>
+  </si>
+  <si>
+    <t>Corresponding</t>
   </si>
 </sst>
 </file>
@@ -439,7 +476,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -613,4 +650,136 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="10" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
<MS 2/16> TestCase id is hard coded excel Iteration.
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -93,34 +93,40 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>987654321</t>
-  </si>
-  <si>
     <t>merlin.samuel@gmail.com</t>
   </si>
   <si>
-    <t>06245678756</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>Austin Woods</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>North</t>
-  </si>
-  <si>
-    <t>90640</t>
-  </si>
-  <si>
-    <t>Merlin</t>
-  </si>
-  <si>
-    <t>Corresponding</t>
+    <t>Line1</t>
+  </si>
+  <si>
+    <t>Line2</t>
+  </si>
+  <si>
+    <t>Line3</t>
+  </si>
+  <si>
+    <t>Line4</t>
+  </si>
+  <si>
+    <t>Line5</t>
+  </si>
+  <si>
+    <t>Line6</t>
+  </si>
+  <si>
+    <t>Line7</t>
+  </si>
+  <si>
+    <t>Line8</t>
+  </si>
+  <si>
+    <t>Line9</t>
+  </si>
+  <si>
+    <t>Line10</t>
+  </si>
+  <si>
+    <t>Line11</t>
   </si>
 </sst>
 </file>
@@ -473,81 +479,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>16</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -558,22 +570,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="10" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="11" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -607,45 +619,51 @@
       <c r="K1" t="s">
         <v>18</v>
       </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -654,10 +672,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,11 +683,9 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="10" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -679,99 +695,27 @@
       <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<MS 2/18> Structured script
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -127,6 +127,30 @@
   </si>
   <si>
     <t>Line11</t>
+  </si>
+  <si>
+    <t>St Patrick Lewis</t>
+  </si>
+  <si>
+    <t>merlinsamuel@gmai.com</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>Merlin</t>
+  </si>
+  <si>
+    <t>7047634589</t>
+  </si>
+  <si>
+    <t>07236254644</t>
+  </si>
+  <si>
+    <t>260</t>
+  </si>
+  <si>
+    <t>90640</t>
   </si>
 </sst>
 </file>
@@ -479,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,6 +584,44 @@
         <v>16</v>
       </c>
       <c r="L2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -570,10 +632,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -661,12 +723,49 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
<MS 2/19> Cross Browser(Ch & FF) With & Without DataProvider
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -506,7 +506,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
<MS 2/23> Excel Data Formatter Code
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Intro_0" sheetId="4" r:id="rId1"/>
-    <sheet name="BD_1" sheetId="1" r:id="rId2"/>
+    <sheet name="SoleTraderDP" sheetId="1" r:id="rId2"/>
     <sheet name="sample" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -93,9 +93,6 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>merlin.samuel@gmail.com</t>
-  </si>
-  <si>
     <t>Line1</t>
   </si>
   <si>
@@ -151,13 +148,163 @@
   </si>
   <si>
     <t>90640</t>
+  </si>
+  <si>
+    <t>Business /Organisation name</t>
+  </si>
+  <si>
+    <t>Business/organisation telephone number</t>
+  </si>
+  <si>
+    <t>Business/organisation e-mail address</t>
+  </si>
+  <si>
+    <t>Mobile number</t>
+  </si>
+  <si>
+    <t>Building name/number</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>Town /City</t>
+  </si>
+  <si>
+    <t>County/State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Post Code</t>
+  </si>
+  <si>
+    <t>Trading Name and/or any other aliases</t>
+  </si>
+  <si>
+    <t>Contact name/department for correspondence</t>
+  </si>
+  <si>
+    <t>Is your trading address different from your registered address?</t>
+  </si>
+  <si>
+    <t>Town/City</t>
+  </si>
+  <si>
+    <t>What address would you like your statements and correspondence sent to?</t>
+  </si>
+  <si>
+    <t>TestCase id</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Patrick Industries</t>
+  </si>
+  <si>
+    <t>Sibley Groove</t>
+  </si>
+  <si>
+    <t>East Ham</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>E12 6SE</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Registered Address</t>
+  </si>
+  <si>
+    <t>NewHam</t>
+  </si>
+  <si>
+    <t>Upton Park</t>
+  </si>
+  <si>
+    <t>TC003</t>
+  </si>
+  <si>
+    <t>Veggie Processing</t>
+  </si>
+  <si>
+    <t>mail2_merlin@yahoo.com</t>
+  </si>
+  <si>
+    <t>07960015047</t>
+  </si>
+  <si>
+    <t>Rosemaid Ave</t>
+  </si>
+  <si>
+    <t>Montere Park</t>
+  </si>
+  <si>
+    <t>Veggie Industries</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Baruch</t>
+  </si>
+  <si>
+    <t>Babyoee</t>
+  </si>
+  <si>
+    <t>Delmare Ave</t>
+  </si>
+  <si>
+    <t>San Gabriel Valley</t>
+  </si>
+  <si>
+    <t>07944226398</t>
+  </si>
+  <si>
+    <t>ms@gmail.com</t>
+  </si>
+  <si>
+    <t>Babyoee Planet</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>EC1A 1BB</t>
+  </si>
+  <si>
+    <t>M1 1AE</t>
+  </si>
+  <si>
+    <t>SE1 8UJ</t>
+  </si>
+  <si>
+    <t>S6 1SW</t>
+  </si>
+  <si>
+    <t>WC1N 3AX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,21 +319,56 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -197,7 +379,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -207,6 +389,40 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -503,130 +719,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="12" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -635,7 +894,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -686,7 +945,7 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -724,36 +983,36 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>6</v>
@@ -771,58 +1030,331 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="6" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" customWidth="1"/>
+    <col min="15" max="20" width="17.5703125" customWidth="1"/>
+    <col min="21" max="21" width="22.5703125" customWidth="1"/>
+    <col min="22" max="27" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
+    <row r="1" spans="1:27" ht="43.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:27">
+      <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="13">
+        <v>7076067764</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="13">
+        <v>260</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O2" s="13"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="13"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:27">
+      <c r="A3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="B3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="13">
+        <v>7049254564</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="13">
+        <v>268</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="O3" s="13">
+        <v>26</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="V3" s="13">
+        <v>32</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="13">
+        <v>7034657240</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="13">
+        <v>249</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="13">
+        <v>40</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="V4" s="13"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
<MS 2/24> Chrome Notification disabled code
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro_0" sheetId="4" r:id="rId1"/>
     <sheet name="SoleTraderDP" sheetId="1" r:id="rId2"/>
     <sheet name="sample" sheetId="5" r:id="rId3"/>
+    <sheet name="FBLogin" sheetId="6" r:id="rId4"/>
+    <sheet name="RedBus" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -295,6 +297,21 @@
   </si>
   <si>
     <t>WC1N 3AX</t>
+  </si>
+  <si>
+    <t>TestCaseid</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PassWord</t>
+  </si>
+  <si>
+    <t>mail2merlin@gmail.com</t>
+  </si>
+  <si>
+    <t>jesus4me</t>
   </si>
 </sst>
 </file>
@@ -721,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1033,7 +1050,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1357,4 +1374,73 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
<MS 3/1> Radio button & Auto Suggest code added in Utility
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="102">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>jesus4me</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Nagercoil</t>
   </si>
 </sst>
 </file>
@@ -396,7 +408,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -440,6 +452,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1381,7 +1396,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1447,14 +1462,65 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34.5" customHeight="1">
+      <c r="A2" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="31.5" customHeight="1">
+      <c r="A3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29.25" customHeight="1">
+      <c r="A4" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
<MS 3/6> Browser separated in library
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13065" windowHeight="2805" tabRatio="710"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="5760" windowHeight="2805" tabRatio="710"/>
   </bookViews>
   <sheets>
     <sheet name="RBS_EOBAO_Status" sheetId="9" r:id="rId1"/>
     <sheet name="IntroPg" sheetId="4" r:id="rId2"/>
-    <sheet name="FB_Login" sheetId="6" r:id="rId3"/>
-    <sheet name="BusinessDetailsPg" sheetId="5" r:id="rId4"/>
-    <sheet name="FB_Status" sheetId="8" r:id="rId5"/>
+    <sheet name="BusinessDetailsPg" sheetId="5" r:id="rId3"/>
+    <sheet name="FB_Status" sheetId="8" r:id="rId4"/>
+    <sheet name="FB_Login" sheetId="6" r:id="rId5"/>
     <sheet name="Redbus_Status" sheetId="10" r:id="rId6"/>
     <sheet name="RedBus_Search" sheetId="7" r:id="rId7"/>
     <sheet name="SoleTraderDP" sheetId="1" r:id="rId8"/>
@@ -338,49 +338,49 @@
     <t>Final Status</t>
   </si>
   <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test@test.com</t>
+  </si>
+  <si>
     <t>Complete</t>
   </si>
   <si>
+    <t>2017_03_06-20.55.21</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.55.41</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.55.44</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.56.08</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.56.31</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.56.33</t>
+  </si>
+  <si>
+    <t>2017_03_06-20.56.57</t>
+  </si>
+  <si>
     <t>Incomplete</t>
   </si>
   <si>
+    <t>2017_03_06-20.57.13</t>
+  </si>
+  <si>
     <t>Fail</t>
   </si>
   <si>
-    <t>2017_03_06-17.31.04</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.31.23</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.31.26</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.31.49</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.32.11</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.32.13</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.32.35</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.32.52</t>
-  </si>
-  <si>
-    <t>2017_03_06-17.32.54</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test@test.com</t>
+    <t>2017_03_06-20.57.15</t>
   </si>
 </sst>
 </file>
@@ -675,6 +675,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -728,9 +731,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1030,7 +1030,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1055,10 +1055,10 @@
       <c r="A2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="29" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1066,10 +1066,10 @@
       <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1077,11 +1077,11 @@
       <c r="A4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="40" t="s">
-        <v>117</v>
+      <c r="B4" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1094,7 +1094,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1187,10 +1187,10 @@
       <c r="L2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" s="24" t="s">
+      <c r="M2" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="N2" s="25" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1231,10 +1231,10 @@
       <c r="L3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="30" t="s">
+      <c r="M3" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="N3" s="31" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1275,10 +1275,10 @@
       <c r="L4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" s="36" t="s">
+      <c r="M4" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="N4" s="37" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1290,89 +1290,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>119</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1540,10 +1461,10 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
-      <c r="AB2" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC2" s="26" t="s">
+      <c r="AB2" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC2" s="27" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1629,10 +1550,10 @@
       <c r="AA3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AB3" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC3" s="32" t="s">
+      <c r="AB3" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC3" s="33" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1704,11 +1625,11 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="AC4" s="38" t="s">
+      <c r="AB4" s="38" t="s">
         <v>116</v>
+      </c>
+      <c r="AC4" s="39" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1722,7 +1643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1768,6 +1689,85 @@
       <c r="C4" s="19"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17.25" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
<MS 3/13> Listener implemented in all 3 packages
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="5760" windowHeight="2805" tabRatio="710"/>
+    <workbookView activeTab="6" firstSheet="1" tabRatio="710" windowHeight="2805" windowWidth="5760" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="RBS_EOBAO_Status" sheetId="9" r:id="rId1"/>
-    <sheet name="IntroPg" sheetId="4" r:id="rId2"/>
-    <sheet name="BusinessDetailsPg" sheetId="5" r:id="rId3"/>
-    <sheet name="FB_Status" sheetId="8" r:id="rId4"/>
-    <sheet name="FB_Login" sheetId="6" r:id="rId5"/>
-    <sheet name="Redbus_Status" sheetId="10" r:id="rId6"/>
-    <sheet name="RedBus_Search" sheetId="7" r:id="rId7"/>
-    <sheet name="SoleTraderDP" sheetId="1" r:id="rId8"/>
+    <sheet name="RBS_EOBAO_Status" r:id="rId1" sheetId="9"/>
+    <sheet name="IntroPg" r:id="rId2" sheetId="4"/>
+    <sheet name="BusinessDetailsPg" r:id="rId3" sheetId="5"/>
+    <sheet name="FB_Status" r:id="rId4" sheetId="8"/>
+    <sheet name="FB_Login" r:id="rId5" sheetId="6"/>
+    <sheet name="Redbus_Status" r:id="rId6" sheetId="10"/>
+    <sheet name="RedBus_Search" r:id="rId7" sheetId="7"/>
+    <sheet name="SoleTraderDP" r:id="rId8" sheetId="1"/>
+    <sheet name="Sample" r:id="rId9" sheetId="11"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="122">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -350,25 +351,43 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>2017_03_11-17.43.24</t>
-  </si>
-  <si>
-    <t>2017_03_11-17.43.43</t>
-  </si>
-  <si>
-    <t>2017_03_11-17.44.18</t>
-  </si>
-  <si>
     <t>Incomplete</t>
   </si>
   <si>
-    <t>2017_03_11-17.44.27</t>
-  </si>
-  <si>
-    <t>2017_03_11-17.44.50</t>
-  </si>
-  <si>
-    <t>2017_03_11-17.45.09</t>
+    <t>2017_03_13-12.08.59</t>
+  </si>
+  <si>
+    <t>2017_03_13-12.09.21</t>
+  </si>
+  <si>
+    <t>2017_03_13-12.12.54</t>
+  </si>
+  <si>
+    <t>2017_03_13-12.13.11</t>
+  </si>
+  <si>
+    <t>2017_03_13-12.30.05</t>
+  </si>
+  <si>
+    <t>2017_03_13-12.30.27</t>
+  </si>
+  <si>
+    <t>mail2merlin@gmail.com</t>
+  </si>
+  <si>
+    <t>jthomas@gmail.com</t>
+  </si>
+  <si>
+    <t>Baruch@1ba</t>
+  </si>
+  <si>
+    <t>2017_03_13-13.51.48</t>
+  </si>
+  <si>
+    <t>2017_03_13-14.16.13</t>
+  </si>
+  <si>
+    <t>2017_03_13-14.20.33</t>
   </si>
 </sst>
 </file>
@@ -378,7 +397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +509,44 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -525,8 +580,18 @@
         <fgColor indexed="10"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -586,123 +651,237 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+  <cellXfs count="43">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyNumberFormat="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyProtection="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="7" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="8" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="10" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="11" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="12" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="13" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="14" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="15" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="4" fontId="16" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="5" fontId="17" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="4" fontId="18" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="5" fontId="19" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="4" fontId="20" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="5" fontId="21" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyBorder="true" applyFill="true" applyFont="true" borderId="14" fillId="4" fontId="22" numFmtId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="14" xfId="0" applyBorder="true" applyFont="true" applyFill="true">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -711,10 +890,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -870,7 +1049,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -879,13 +1058,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -895,7 +1074,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -904,7 +1083,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -913,7 +1092,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -923,12 +1102,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -959,7 +1138,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -978,7 +1157,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -993,51 +1172,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row customHeight="1" ht="18" r="1" spans="1:3">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="24"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1051,54 +1230,54 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1139,11 +1318,11 @@
       <c r="L2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N2" s="26" t="s">
-        <v>109</v>
+      <c r="N2" s="23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1183,10 +1362,10 @@
       <c r="L3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="31" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1227,15 +1406,15 @@
       <c r="L4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="N4" s="30" t="s">
-        <v>111</v>
+      <c r="N4" s="27" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -1244,114 +1423,114 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Z15" sqref="Z15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="11" width="22" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="29.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="20" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="22.5703125" customWidth="1" collapsed="1"/>
-    <col min="22" max="27" width="14.85546875" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.5703125" collapsed="true"/>
+    <col min="6" max="11" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="27.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="29.7109375" collapsed="true"/>
+    <col min="15" max="20" customWidth="true" width="17.5703125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="22" max="27" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="43.5" customHeight="1">
-      <c r="A1" s="20" t="s">
+    <row customHeight="1" ht="43.5" r="1" spans="1:29">
+      <c r="A1" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="O1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="P1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="21" t="s">
+      <c r="R1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="21" t="s">
+      <c r="T1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="21" t="s">
+      <c r="V1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="21" t="s">
+      <c r="W1" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="21" t="s">
+      <c r="X1" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="21" t="s">
+      <c r="Y1" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="21" t="s">
+      <c r="Z1" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AA1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AB1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AC1" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1395,7 +1574,7 @@
       <c r="M2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="16" t="s">
         <v>61</v>
       </c>
       <c r="O2" s="10"/>
@@ -1413,11 +1592,11 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="AC2" s="28" t="s">
-        <v>110</v>
+      <c r="AC2" s="25" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -1460,7 +1639,7 @@
       <c r="M3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="N3" s="19" t="s">
+      <c r="N3" s="16" t="s">
         <v>67</v>
       </c>
       <c r="O3" s="10">
@@ -1502,10 +1681,10 @@
       <c r="AA3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="AC3" s="36" t="s">
+      <c r="AC3" s="33" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1549,7 +1728,7 @@
       <c r="M4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="N4" s="19"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="10">
         <v>40</v>
       </c>
@@ -1577,20 +1756,20 @@
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
-      <c r="AB4" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="AC4" s="32" t="s">
+      <c r="AB4" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC4" s="29" t="s">
         <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D3"/>
+    <hyperlink r:id="rId3" ref="D4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
@@ -1605,8 +1784,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1621,27 +1800,27 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1649,18 +1828,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1">
+    <row customHeight="1" ht="17.25" r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>93</v>
       </c>
@@ -1670,10 +1851,10 @@
       <c r="C1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1681,48 +1862,53 @@
       <c r="A2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>106</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="D2" s="34"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row customHeight="1" ht="19.5" r="3" spans="1:5">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>74</v>
+      <c r="B3" s="19" t="s">
+        <v>116</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="D3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
+      <c r="B4" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="35"/>
+      <c r="E4" s="36"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink r:id="rId1" ref="B2"/>
+    <hyperlink r:id="rId2" ref="B3"/>
+    <hyperlink r:id="rId3" ref="B4"/>
+    <hyperlink r:id="rId4" ref="C4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1736,8 +1922,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1752,46 +1938,48 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="15"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="7" t="s">
         <v>93</v>
       </c>
@@ -1802,7 +1990,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34.5" customHeight="1">
+    <row customHeight="1" ht="34.5" r="2" spans="1:5">
       <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
@@ -1812,8 +2000,14 @@
       <c r="C2" s="13" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="31.5" customHeight="1">
+      <c r="D2" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" t="s" s="42">
+        <v>121</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="31.5" r="3" spans="1:5">
       <c r="A3" s="13" t="s">
         <v>24</v>
       </c>
@@ -1824,7 +2018,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29.25" customHeight="1">
+    <row customHeight="1" ht="29.25" r="4" spans="1:5">
       <c r="A4" s="13" t="s">
         <v>72</v>
       </c>
@@ -1836,7 +2030,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
@@ -1851,11 +2045,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="11" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="6" max="11" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1972,10 +2166,26 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="D2"/>
+    <hyperlink r:id="rId2" ref="D3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" style="11" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
<MS 3/15> Listener and Extent Reports combined.
</commit_message>
<xml_diff>
--- a/ExcelData/ST_datasheet.xlsx
+++ b/ExcelData/ST_datasheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="5760" windowHeight="2805" tabRatio="710"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="5760" windowHeight="2805" tabRatio="774" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RBS_EOBAO_Status" sheetId="9" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="143">
   <si>
     <t>test.test@test.com</t>
   </si>
@@ -237,9 +237,6 @@
     <t>Upton Park</t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
     <t>Veggie Processing</t>
   </si>
   <si>
@@ -330,85 +327,130 @@
     <t>test@test.com</t>
   </si>
   <si>
+    <t>mail2merlin@gmail.com</t>
+  </si>
+  <si>
+    <t>jthomas@gmail.com</t>
+  </si>
+  <si>
+    <t>Baruch@1ba</t>
+  </si>
+  <si>
+    <t>S.No</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>TestCase Name</t>
+  </si>
+  <si>
+    <t>TestData id</t>
+  </si>
+  <si>
+    <t>TestDataid</t>
+  </si>
+  <si>
+    <t>TD001</t>
+  </si>
+  <si>
+    <t>TD002</t>
+  </si>
+  <si>
+    <t>TD003</t>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:24:29</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:24:49</t>
+  </si>
+  <si>
+    <t>RBS_ST1</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:24:51</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:25:13</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:25:28</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:25:29</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:25:50</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:26:09</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:26:10</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:28:41</t>
+  </si>
+  <si>
+    <t>FB_Login</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:28:47</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:32:05</t>
+  </si>
+  <si>
+    <t>Redbus_Search</t>
+  </si>
+  <si>
+    <t>2017-03-15 04:32:08</t>
+  </si>
+  <si>
+    <t>Class1</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:20:46</t>
+  </si>
+  <si>
+    <t>Class2</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:20:48</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:23:16</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:23:18</t>
+  </si>
+  <si>
+    <t>Class3</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:23:19</t>
+  </si>
+  <si>
+    <t>Class4</t>
+  </si>
+  <si>
+    <t>2017-03-15 05:23:20</t>
+  </si>
+  <si>
     <t>jesus4me</t>
-  </si>
-  <si>
-    <t>mail2merlin@gmail.com</t>
-  </si>
-  <si>
-    <t>jthomas@gmail.com</t>
-  </si>
-  <si>
-    <t>Baruch@1ba</t>
-  </si>
-  <si>
-    <t>S.No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>TestCase Name</t>
-  </si>
-  <si>
-    <t>TestData id</t>
-  </si>
-  <si>
-    <t>TestDataid</t>
-  </si>
-  <si>
-    <t>Class1</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.35.35</t>
-  </si>
-  <si>
-    <t>Class2</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.35.36</t>
-  </si>
-  <si>
-    <t>Class3</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.35.37</t>
-  </si>
-  <si>
-    <t>Class4</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.36.15</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.36.34</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.37.01</t>
-  </si>
-  <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.37.10</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.37.32</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.37.51</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.39.17</t>
-  </si>
-  <si>
-    <t>2017_03_14-01.40.10</t>
   </si>
 </sst>
 </file>
@@ -418,7 +460,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="76">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -442,6 +484,240 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -681,7 +957,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -736,8 +1012,51 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -764,7 +1083,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -815,14 +1134,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -838,100 +1152,222 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="57" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="62" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="65" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="70" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="74" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1231,69 +1667,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>107</v>
+      <c r="D2" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>107</v>
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>107</v>
+      <c r="B4" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="61" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1306,7 +1773,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N1" sqref="A1:N1"/>
+      <selection activeCell="M4" sqref="M4:N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1319,52 +1786,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="N1" s="22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="11" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>7</v>
@@ -1396,19 +1863,19 @@
       <c r="K2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="44" t="s">
-        <v>120</v>
+      <c r="M2" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>7</v>
@@ -1440,19 +1907,19 @@
       <c r="K3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="N3" s="52" t="s">
-        <v>125</v>
+      <c r="M3" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="N3" s="55" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="11" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>7</v>
@@ -1484,14 +1951,14 @@
       <c r="K4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="N4" s="48" t="s">
-        <v>122</v>
+      <c r="M4" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="N4" s="47" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1504,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:AC1"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1527,97 +1994,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="43.5" customHeight="1">
-      <c r="A1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="L1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="22" t="s">
+      <c r="M1" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="22" t="s">
+      <c r="N1" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="P1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="Q1" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="R1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="S1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="25" t="s">
+      <c r="T1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="W1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="Y1" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="Z1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AA1" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="AB1" s="22" t="s">
+      <c r="AB1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC1" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="AC1" s="22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>36</v>
@@ -1644,10 +2111,10 @@
         <v>59</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>61</v>
@@ -1672,53 +2139,53 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
-      <c r="AA2" s="23"/>
-      <c r="AB2" s="45" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC2" s="46" t="s">
-        <v>121</v>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC2" s="41" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="9">
         <v>7049254564</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="F3" s="9">
         <v>268</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>59</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="L3" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>77</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="N3" s="13" t="s">
         <v>66</v>
@@ -1739,7 +2206,7 @@
         <v>38</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U3" s="4" t="s">
         <v>67</v>
@@ -1759,55 +2226,55 @@
       <c r="Z3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AA3" s="23" t="s">
+      <c r="AA3" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="AB3" s="53" t="s">
-        <v>119</v>
-      </c>
-      <c r="AC3" s="54" t="s">
-        <v>126</v>
+      <c r="AB3" s="56" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC3" s="57" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="7" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4" s="9">
         <v>7034657240</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="9">
         <v>265</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>59</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N4" s="13"/>
       <c r="O4" s="9">
@@ -1826,7 +2293,7 @@
         <v>38</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U4" s="4" t="s">
         <v>68</v>
@@ -1836,12 +2303,12 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
       <c r="Z4" s="4"/>
-      <c r="AA4" s="23"/>
-      <c r="AB4" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="AC4" s="50" t="s">
-        <v>124</v>
+      <c r="AA4" s="20"/>
+      <c r="AB4" s="48" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC4" s="49" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1860,7 +2327,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1869,59 +2336,71 @@
     <col min="2" max="2" width="19.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21.75" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>107</v>
+    </row>
+    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="67" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1933,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1947,61 +2426,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A1" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>98</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>109</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="19.5" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>110</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D3" s="55" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="56" t="s">
-        <v>127</v>
+        <v>101</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="62" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="63" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="7" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="17"/>
@@ -2012,6 +2491,7 @@
     <hyperlink ref="B3" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId5" display="Baruch@1ba"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2022,7 +2502,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2031,59 +2511,71 @@
     <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="16.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>107</v>
+    </row>
+    <row r="2" spans="1:5" ht="21" customHeight="1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="71" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" s="73" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2588,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2109,59 +2601,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19.5" customHeight="1">
+      <c r="A2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="22" t="s">
+      <c r="B3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="19.5" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="C3" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="12" t="s">
+      <c r="D3" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A4" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2314,7 +2806,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2328,132 +2820,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="30" t="s">
-        <v>113</v>
+      <c r="B2" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>115</v>
+      <c r="A3" s="24"/>
+      <c r="B3" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="80" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="81" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="84" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="85" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="87" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="38" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>112</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>117</v>
+      <c r="E5" s="89" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="90" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="93" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="10" t="s">
-        <v>107</v>
+      <c r="A7" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="97" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="A8" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="A9" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="A10" s="25"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>